<commit_message>
Add numberOfLikes and crowdControlRisk fields to class Talk
</commit_message>
<xml_diff>
--- a/optaplanner-examples/data/conferencescheduling/unsolved/36talks-12timeslots-5rooms.xlsx
+++ b/optaplanner-examples/data/conferencescheduling/unsolved/36talks-12timeslots-5rooms.xlsx
@@ -25,6 +25,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments10.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C3" authorId="0">
+      <text>
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
+PINNED BY USER
+</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/comments11.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
@@ -33,11 +51,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -53,11 +69,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -73,11 +87,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -93,11 +105,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -113,11 +123,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -131,13 +139,11 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0">
+    <comment ref="C18" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -153,11 +159,9 @@
   <commentList>
     <comment ref="C3" authorId="0">
       <text>
-        <t xml:space="preserve">S14: Troubleshooting reliable RestEasy
-    Amy Green
+        <t xml:space="preserve">S31: Understand mobile Angular
+    Flo Poe
 PINNED BY USER
--1hard total
-    -1hard for 1 Speaker unavailable timeslots
 </t>
       </text>
     </comment>
@@ -166,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2309" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="289">
   <si>
     <t>Conference name</t>
   </si>
@@ -591,6 +595,12 @@
     <t>Prerequisite talks codes</t>
   </si>
   <si>
+    <t>Number of likes</t>
+  </si>
+  <si>
+    <t>Crowd control risk</t>
+  </si>
+  <si>
     <t>Pinned by user</t>
   </si>
   <si>
@@ -627,301 +637,298 @@
     <t>Advanced containerized WildFly</t>
   </si>
   <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>Programmers</t>
+  </si>
+  <si>
+    <t>WildFly</t>
+  </si>
+  <si>
+    <t>S02</t>
+  </si>
+  <si>
+    <t>Learn virtualized Spring</t>
+  </si>
+  <si>
+    <t>Dan Jones, Elsa King</t>
+  </si>
+  <si>
+    <t>Modern Web, IoT</t>
+  </si>
+  <si>
+    <t>Spring</t>
+  </si>
+  <si>
+    <t>S03</t>
+  </si>
+  <si>
+    <t>Intro to serverless Drools</t>
+  </si>
+  <si>
+    <t>Modern Web</t>
+  </si>
+  <si>
+    <t>Business analysts</t>
+  </si>
+  <si>
+    <t>Drools</t>
+  </si>
+  <si>
+    <t>S04</t>
+  </si>
+  <si>
+    <t>Discover AI-driven OptaPlanner</t>
+  </si>
+  <si>
+    <t>Gus Poe, Hugo Rye</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>OptaPlanner</t>
+  </si>
+  <si>
+    <t>S05</t>
+  </si>
+  <si>
+    <t>Mastering machine learning jBPM</t>
+  </si>
+  <si>
+    <t>IoT</t>
+  </si>
+  <si>
+    <t>jBPM</t>
+  </si>
+  <si>
+    <t>S06</t>
+  </si>
+  <si>
+    <t>Tuning IOT-driven Camel</t>
+  </si>
+  <si>
+    <t>Camel</t>
+  </si>
+  <si>
+    <t>S07</t>
+  </si>
+  <si>
+    <t>Building deep learning XStream</t>
+  </si>
+  <si>
+    <t>XStream</t>
+  </si>
+  <si>
+    <t>S08</t>
+  </si>
+  <si>
+    <t>Securing scalable Docker</t>
+  </si>
+  <si>
+    <t>Docker, Kubernetes</t>
+  </si>
+  <si>
+    <t>S09</t>
+  </si>
+  <si>
+    <t>Debug enterprise Hibernate</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Hibernate</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>Prepare for streaming GWT</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>GWT</t>
+  </si>
+  <si>
+    <t>S11</t>
+  </si>
+  <si>
+    <t>Understand mobile Errai</t>
+  </si>
+  <si>
+    <t>Cloud, Big Data</t>
+  </si>
+  <si>
+    <t>Errai</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>Applying modern Angular</t>
+  </si>
+  <si>
+    <t>Flo Poe, Gus Rye, Hugo Smith</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>S13</t>
+  </si>
+  <si>
+    <t>Grok distributed Weld</t>
+  </si>
+  <si>
     <t>Middleware</t>
   </si>
   <si>
-    <t>Programmers</t>
-  </si>
-  <si>
-    <t>WildFly</t>
-  </si>
-  <si>
-    <t>S02</t>
-  </si>
-  <si>
-    <t>Learn virtualized Spring</t>
-  </si>
-  <si>
-    <t>Dan Jones, Elsa King</t>
+    <t>Weld</t>
+  </si>
+  <si>
+    <t>S14</t>
+  </si>
+  <si>
+    <t>Troubleshooting reliable RestEasy</t>
+  </si>
+  <si>
+    <t>Middleware, IoT</t>
+  </si>
+  <si>
+    <t>RestEasy</t>
+  </si>
+  <si>
+    <t>S15</t>
+  </si>
+  <si>
+    <t>Using secure Android</t>
+  </si>
+  <si>
+    <t>Big Data, Cloud</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>S16</t>
+  </si>
+  <si>
+    <t>Deliver stable Tensorflow</t>
+  </si>
+  <si>
+    <t>Beth Jones, Chad King</t>
+  </si>
+  <si>
+    <t>Tensorflow</t>
+  </si>
+  <si>
+    <t>S17</t>
+  </si>
+  <si>
+    <t>Implement platform-independent VertX</t>
+  </si>
+  <si>
+    <t>VertX</t>
+  </si>
+  <si>
+    <t>S18</t>
+  </si>
+  <si>
+    <t>Program flexible JUnit</t>
+  </si>
+  <si>
+    <t>Modern Web, Big Data</t>
+  </si>
+  <si>
+    <t>JUnit</t>
+  </si>
+  <si>
+    <t>S19</t>
+  </si>
+  <si>
+    <t>Hack modularized Keycloak</t>
+  </si>
+  <si>
+    <t>Beth Fox, Chad Green</t>
   </si>
   <si>
     <t>Culture</t>
   </si>
   <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>S03</t>
-  </si>
-  <si>
-    <t>Intro to serverless Drools</t>
-  </si>
-  <si>
-    <t>Drools</t>
-  </si>
-  <si>
-    <t>S04</t>
-  </si>
-  <si>
-    <t>Discover AI-driven OptaPlanner</t>
-  </si>
-  <si>
-    <t>Big Data</t>
-  </si>
-  <si>
-    <t>OptaPlanner</t>
-  </si>
-  <si>
-    <t>S05</t>
-  </si>
-  <si>
-    <t>Mastering machine learning jBPM</t>
-  </si>
-  <si>
-    <t>Hugo Rye, Ivy Smith</t>
-  </si>
-  <si>
-    <t>Cloud, Big Data</t>
-  </si>
-  <si>
-    <t>Business analysts</t>
-  </si>
-  <si>
-    <t>jBPM</t>
-  </si>
-  <si>
-    <t>S06</t>
-  </si>
-  <si>
-    <t>Tuning IOT-driven Camel</t>
-  </si>
-  <si>
-    <t>IoT</t>
-  </si>
-  <si>
-    <t>Camel</t>
-  </si>
-  <si>
-    <t>S07</t>
-  </si>
-  <si>
-    <t>Building deep learning XStream</t>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Keycloak</t>
+  </si>
+  <si>
+    <t>S20</t>
+  </si>
+  <si>
+    <t>Hands on real-time WildFly</t>
+  </si>
+  <si>
+    <t>S21</t>
+  </si>
+  <si>
+    <t>Advanced containerized Spring</t>
+  </si>
+  <si>
+    <t>Financial services</t>
+  </si>
+  <si>
+    <t>S22</t>
+  </si>
+  <si>
+    <t>Learn virtualized Drools</t>
+  </si>
+  <si>
+    <t>S23</t>
+  </si>
+  <si>
+    <t>Intro to serverless OptaPlanner</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>S24</t>
+  </si>
+  <si>
+    <t>Discover AI-driven jBPM</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>S25</t>
+  </si>
+  <si>
+    <t>Mastering machine learning Camel</t>
+  </si>
+  <si>
+    <t>S26</t>
+  </si>
+  <si>
+    <t>Tuning IOT-driven XStream</t>
+  </si>
+  <si>
+    <t>S27</t>
+  </si>
+  <si>
+    <t>Building deep learning Docker</t>
   </si>
   <si>
     <t>Amy Fox, Beth Green</t>
   </si>
   <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>XStream</t>
-  </si>
-  <si>
-    <t>S08</t>
-  </si>
-  <si>
-    <t>Securing scalable Docker</t>
-  </si>
-  <si>
-    <t>Chad Jones, Dan King</t>
-  </si>
-  <si>
-    <t>Security</t>
-  </si>
-  <si>
-    <t>Docker, Kubernetes</t>
-  </si>
-  <si>
-    <t>S09</t>
-  </si>
-  <si>
-    <t>Debug enterprise Hibernate</t>
-  </si>
-  <si>
-    <t>Middleware, Cloud</t>
-  </si>
-  <si>
-    <t>Hibernate</t>
-  </si>
-  <si>
-    <t>S10</t>
-  </si>
-  <si>
-    <t>Prepare for streaming GWT</t>
-  </si>
-  <si>
-    <t>Culture, Mobile</t>
-  </si>
-  <si>
-    <t>GWT</t>
-  </si>
-  <si>
-    <t>S11</t>
-  </si>
-  <si>
-    <t>Understand mobile Errai</t>
-  </si>
-  <si>
-    <t>Gus Rye, Hugo Smith</t>
-  </si>
-  <si>
-    <t>IoT, Modern Web</t>
-  </si>
-  <si>
-    <t>Financial services</t>
-  </si>
-  <si>
-    <t>Errai</t>
-  </si>
-  <si>
-    <t>S12</t>
-  </si>
-  <si>
-    <t>Applying modern Angular</t>
-  </si>
-  <si>
-    <t>Modern Web</t>
-  </si>
-  <si>
-    <t>Government</t>
-  </si>
-  <si>
-    <t>Angular</t>
-  </si>
-  <si>
-    <t>S13</t>
-  </si>
-  <si>
-    <t>Grok distributed Weld</t>
-  </si>
-  <si>
-    <t>Weld</t>
-  </si>
-  <si>
-    <t>S14</t>
-  </si>
-  <si>
-    <t>Troubleshooting reliable RestEasy</t>
-  </si>
-  <si>
-    <t>RestEasy</t>
-  </si>
-  <si>
-    <t>S15</t>
-  </si>
-  <si>
-    <t>Using secure Android</t>
-  </si>
-  <si>
-    <t>Cloud</t>
-  </si>
-  <si>
-    <t>Android</t>
-  </si>
-  <si>
-    <t>S16</t>
-  </si>
-  <si>
-    <t>Deliver stable Tensorflow</t>
-  </si>
-  <si>
-    <t>Modern Web, Culture</t>
-  </si>
-  <si>
-    <t>Tensorflow</t>
-  </si>
-  <si>
-    <t>S17</t>
-  </si>
-  <si>
-    <t>Implement platform-independent VertX</t>
-  </si>
-  <si>
-    <t>VertX</t>
-  </si>
-  <si>
-    <t>S18</t>
-  </si>
-  <si>
-    <t>Program flexible JUnit</t>
-  </si>
-  <si>
-    <t>JUnit</t>
-  </si>
-  <si>
-    <t>S19</t>
-  </si>
-  <si>
-    <t>Hack modularized Keycloak</t>
-  </si>
-  <si>
-    <t>Keycloak</t>
-  </si>
-  <si>
-    <t>S20</t>
-  </si>
-  <si>
-    <t>Hands on real-time WildFly</t>
-  </si>
-  <si>
-    <t>S21</t>
-  </si>
-  <si>
-    <t>Advanced containerized Spring</t>
-  </si>
-  <si>
-    <t>Artificial Intelligence, Culture</t>
-  </si>
-  <si>
-    <t>S22</t>
-  </si>
-  <si>
-    <t>Learn virtualized Drools</t>
-  </si>
-  <si>
-    <t>Education</t>
-  </si>
-  <si>
-    <t>S23</t>
-  </si>
-  <si>
-    <t>Intro to serverless OptaPlanner</t>
-  </si>
-  <si>
-    <t>Culture, Security</t>
-  </si>
-  <si>
-    <t>S24</t>
-  </si>
-  <si>
-    <t>Discover AI-driven jBPM</t>
-  </si>
-  <si>
-    <t>Ivy Smith, Jay Watt</t>
-  </si>
-  <si>
     <t>Transportation</t>
   </si>
   <si>
-    <t>S25</t>
-  </si>
-  <si>
-    <t>Mastering machine learning Camel</t>
-  </si>
-  <si>
-    <t>S26</t>
-  </si>
-  <si>
-    <t>Tuning IOT-driven XStream</t>
-  </si>
-  <si>
-    <t>Beth Green, Chad Jones</t>
-  </si>
-  <si>
-    <t>S27</t>
-  </si>
-  <si>
-    <t>Building deep learning Docker</t>
+    <t>Docker</t>
   </si>
   <si>
     <t>S28</t>
@@ -930,9 +937,6 @@
     <t>Securing scalable Hibernate</t>
   </si>
   <si>
-    <t>Elsa Li, Flo Poe</t>
-  </si>
-  <si>
     <t>S29</t>
   </si>
   <si>
@@ -951,28 +955,19 @@
     <t>Understand mobile Angular</t>
   </si>
   <si>
-    <t>Ivy Watt, Jay Cole</t>
-  </si>
-  <si>
     <t>S32</t>
   </si>
   <si>
     <t>Applying modern Weld</t>
   </si>
   <si>
-    <t>Amy Green, Beth Jones</t>
-  </si>
-  <si>
     <t>S33</t>
   </si>
   <si>
     <t>Grok distributed RestEasy</t>
   </si>
   <si>
-    <t>Chad King, Dan Li</t>
-  </si>
-  <si>
-    <t>Security, Culture</t>
+    <t>Hugo Smith, Ivy Watt</t>
   </si>
   <si>
     <t>S34</t>
@@ -981,22 +976,16 @@
     <t>Troubleshooting reliable Android</t>
   </si>
   <si>
-    <t>Mobile, Cloud</t>
-  </si>
-  <si>
     <t>S35</t>
   </si>
   <si>
     <t>Using secure Tensorflow</t>
   </si>
   <si>
-    <t>Beth Fox, Chad Green</t>
-  </si>
-  <si>
     <t>Score</t>
   </si>
   <si>
-    <t>-70init/-1hard</t>
+    <t>-70init</t>
   </si>
   <si>
     <t>Count</t>
@@ -1014,14 +1003,14 @@
     <t>Total</t>
   </si>
   <si>
-    <t>S14: Troubleshooting reliable RestEasy
-  Amy Green</t>
+    <t>S31: Understand mobile Angular
+  Flo Poe</t>
   </si>
   <si>
     <t>Speaker</t>
   </si>
   <si>
-    <t>S14 @ R 1</t>
+    <t>S31 @ R 1</t>
   </si>
   <si>
     <t>Theme track tag</t>
@@ -1039,7 +1028,7 @@
     <t>Content tag</t>
   </si>
   <si>
-    <t>S14 (level 2)</t>
+    <t>S31 (level 2)</t>
   </si>
   <si>
     <t>Constraint match</t>
@@ -1049,12 +1038,6 @@
   </si>
   <si>
     <t>Total score</t>
-  </si>
-  <si>
-    <t>-1hard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    S14</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1617,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.94140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="22.44140625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
@@ -1692,7 +1675,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -1729,6 +1712,47 @@
       </c>
       <c r="M2" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="3" ht="15.0" customHeight="true">
+      <c r="A3" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1738,6 +1762,7 @@
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1755,7 +1780,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="15.99609375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.6171875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.6171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.6171875" customWidth="true" bestFit="true"/>
@@ -1813,7 +1838,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -1854,13 +1879,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>
@@ -2017,13 +2042,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>
@@ -2139,7 +2164,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -2180,13 +2205,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>
@@ -2343,13 +2368,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>
@@ -2382,10 +2407,10 @@
         <v>72</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2413,7 +2438,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="31.4140625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="19.0703125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.73828125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.66015625" customWidth="true" bestFit="true"/>
   </cols>
@@ -2421,33 +2446,14 @@
     <row r="1"/>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+        <v>288</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -4815,9 +4821,9 @@
     <col min="1" max="1" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="37.3125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="10.78515625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="22.8671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="27.7109375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.30859375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="28.3515625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="21.6953125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="20.05859375" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="17.34375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="16.3046875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="21.8046875" customWidth="true" bestFit="true"/>
@@ -4832,11 +4838,13 @@
     <col min="18" max="18" width="22.84375" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="31.2734375" customWidth="true" bestFit="true"/>
     <col min="20" max="20" width="26.23046875" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="16.65234375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.14453125" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="6.3984375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="6.32421875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="7.02734375" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="17.5390625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="20.140625" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.65234375" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.14453125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="6.3984375" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="6.32421875" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="7.02734375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4907,45 +4915,51 @@
         <v>142</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Y1" s="1" t="s">
-        <v>143</v>
+      <c r="AA1" s="1" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H2" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>72</v>
@@ -4977,28 +4991,34 @@
       <c r="T2" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U2" s="2" t="b">
+      <c r="U2" s="2" t="n">
+        <v>639.0</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X2" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>71</v>
@@ -5007,99 +5027,105 @@
         <v>107</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H3" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>357.0</v>
+      </c>
+      <c r="V3" s="2" t="n">
         <v>2.0</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U3" s="2" t="b">
+      <c r="W3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X3" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>72</v>
@@ -5131,28 +5157,34 @@
       <c r="T4" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U4" s="2" t="b">
+      <c r="U4" s="2" t="n">
+        <v>945.0</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X4" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>71</v>
@@ -5161,22 +5193,22 @@
         <v>110</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="H5" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>72</v>
@@ -5208,52 +5240,58 @@
       <c r="T5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U5" s="2" t="b">
+      <c r="U5" s="2" t="n">
+        <v>325.0</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X5" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA5" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>72</v>
@@ -5285,105 +5323,117 @@
       <c r="T6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U6" s="2" t="b">
+      <c r="U6" s="2" t="n">
+        <v>724.0</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X6" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>170</v>
+        <v>113</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="H7" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U7" s="2" t="n">
+        <v>259.0</v>
+      </c>
+      <c r="V7" s="2" t="n">
         <v>1.0</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U7" s="2" t="b">
+      <c r="W7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X7" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA7" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>74</v>
@@ -5392,22 +5442,22 @@
         <v>114</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="H8" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>72</v>
@@ -5439,52 +5489,58 @@
       <c r="T8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U8" s="2" t="b">
+      <c r="U8" s="2" t="n">
+        <v>500.0</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X8" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA8" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>180</v>
+        <v>115</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H9" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>182</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>72</v>
@@ -5516,19 +5572,25 @@
       <c r="T9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U9" s="2" t="b">
+      <c r="U9" s="2" t="n">
+        <v>558.0</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V9" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X9" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA9" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5543,25 +5605,25 @@
         <v>74</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="H10" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>72</v>
@@ -5593,52 +5655,58 @@
       <c r="T10" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U10" s="2" t="b">
+      <c r="U10" s="2" t="n">
+        <v>264.0</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA10" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H11" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>72</v>
@@ -5670,52 +5738,58 @@
       <c r="T11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U11" s="2" t="b">
+      <c r="U11" s="2" t="n">
+        <v>144.0</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W11" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X11" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA11" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>72</v>
+        <v>192</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>72</v>
@@ -5747,52 +5821,58 @@
       <c r="T12" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U12" s="2" t="b">
+      <c r="U12" s="2" t="n">
+        <v>840.0</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X12" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA12" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>198</v>
+        <v>119</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H13" s="2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>72</v>
@@ -5824,206 +5904,224 @@
       <c r="T13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U13" s="2" t="b">
+      <c r="U13" s="2" t="n">
+        <v>201.0</v>
+      </c>
+      <c r="V13" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W13" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X13" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA13" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>123</v>
+        <v>200</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>205</v>
+        <v>72</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H14" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U14" s="2" t="n">
+        <v>543.0</v>
+      </c>
+      <c r="V14" s="2" t="n">
         <v>2.0</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U14" s="2" t="b">
+      <c r="W14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V14" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X14" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA14" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="H15" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U15" s="2" t="n">
+        <v>973.0</v>
+      </c>
+      <c r="V15" s="2" t="n">
         <v>1.0</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U15" s="2" t="b">
+      <c r="W15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X15" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA15" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>153</v>
+        <v>208</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H16" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>72</v>
@@ -6055,52 +6153,58 @@
       <c r="T16" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U16" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>69</v>
+      <c r="U16" s="2" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="V16" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W16" s="2" t="b">
+        <v>0</v>
       </c>
       <c r="X16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>90</v>
+        <v>72</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA16" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H17" s="2" t="n">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>72</v>
@@ -6132,105 +6236,117 @@
       <c r="T17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U17" s="2" t="b">
+      <c r="U17" s="2" t="n">
+        <v>871.0</v>
+      </c>
+      <c r="V17" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA17" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>219</v>
+        <v>165</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H18" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U18" s="2" t="n">
+        <v>411.0</v>
+      </c>
+      <c r="V18" s="2" t="n">
         <v>3.0</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U18" s="2" t="b">
+      <c r="W18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V18" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA18" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>74</v>
@@ -6239,22 +6355,22 @@
         <v>128</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H19" s="2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>72</v>
@@ -6286,52 +6402,58 @@
       <c r="T19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U19" s="2" t="b">
+      <c r="U19" s="2" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V19" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W19" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA19" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>146</v>
+        <v>105</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>181</v>
+        <v>223</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H20" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>72</v>
@@ -6363,52 +6485,58 @@
       <c r="T20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U20" s="2" t="b">
+      <c r="U20" s="2" t="n">
+        <v>320.0</v>
+      </c>
+      <c r="V20" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W20" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X20" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA20" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>229</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H21" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>72</v>
@@ -6440,52 +6568,58 @@
       <c r="T21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U21" s="2" t="b">
+      <c r="U21" s="2" t="n">
+        <v>142.0</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W21" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V21" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W21" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z21" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA21" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>159</v>
+        <v>228</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>72</v>
@@ -6517,129 +6651,141 @@
       <c r="T22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U22" s="2" t="b">
+      <c r="U22" s="2" t="n">
+        <v>287.0</v>
+      </c>
+      <c r="V22" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V22" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W22" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X22" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA22" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>234</v>
+        <v>175</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>172</v>
+        <v>150</v>
       </c>
       <c r="H23" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U23" s="2" t="n">
+        <v>435.0</v>
+      </c>
+      <c r="V23" s="2" t="n">
         <v>3.0</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U23" s="2" t="b">
+      <c r="W23" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W23" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X23" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA23" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>237</v>
+        <v>72</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>72</v>
@@ -6671,19 +6817,25 @@
       <c r="T24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U24" s="2" t="b">
+      <c r="U24" s="2" t="n">
+        <v>162.0</v>
+      </c>
+      <c r="V24" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V24" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W24" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA24" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -6698,25 +6850,25 @@
         <v>74</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="G25" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H25" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="H25" s="2" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>167</v>
-      </c>
       <c r="J25" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>72</v>
@@ -6748,19 +6900,25 @@
       <c r="T25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U25" s="2" t="b">
+      <c r="U25" s="2" t="n">
+        <v>357.0</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V25" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W25" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA25" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -6775,25 +6933,25 @@
         <v>74</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H26" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>72</v>
@@ -6825,52 +6983,58 @@
       <c r="T26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U26" s="2" t="b">
+      <c r="U26" s="2" t="n">
+        <v>133.0</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V26" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W26" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X26" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA26" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>200</v>
+        <v>72</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="H27" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>72</v>
@@ -6902,43 +7066,49 @@
       <c r="T27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U27" s="2" t="b">
+      <c r="U27" s="2" t="n">
+        <v>915.0</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W27" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA27" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>248</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>249</v>
+        <v>114</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>1.0</v>
@@ -6947,7 +7117,7 @@
         <v>182</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>72</v>
@@ -6979,52 +7149,58 @@
       <c r="T28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U28" s="2" t="b">
+      <c r="U28" s="2" t="n">
+        <v>371.0</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W28" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W28" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X28" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA28" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>118</v>
+        <v>250</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>204</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>72</v>
+        <v>251</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H29" s="2" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>187</v>
+        <v>252</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>72</v>
@@ -7056,96 +7232,108 @@
       <c r="T29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U29" s="2" t="b">
+      <c r="U29" s="2" t="n">
+        <v>551.0</v>
+      </c>
+      <c r="V29" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W29" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X29" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA29" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H30" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="R30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="T30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="U30" s="2" t="n">
+        <v>307.0</v>
+      </c>
+      <c r="V30" s="2" t="n">
         <v>1.0</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="L30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="N30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="T30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="U30" s="2" t="b">
+      <c r="W30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W30" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X30" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA30" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7160,25 +7348,25 @@
         <v>74</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>153</v>
+        <v>228</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="H31" s="2" t="n">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>72</v>
@@ -7210,19 +7398,25 @@
       <c r="T31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U31" s="2" t="b">
+      <c r="U31" s="2" t="n">
+        <v>539.0</v>
+      </c>
+      <c r="V31" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V31" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W31" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X31" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z31" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA31" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7237,25 +7431,25 @@
         <v>74</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>176</v>
+        <v>204</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H32" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>72</v>
@@ -7287,19 +7481,25 @@
       <c r="T32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U32" s="2" t="b">
+      <c r="U32" s="2" t="n">
+        <v>313.0</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W32" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X32" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA32" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7314,25 +7514,25 @@
         <v>74</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>261</v>
+        <v>120</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>72</v>
+        <v>240</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H33" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>72</v>
@@ -7364,52 +7564,58 @@
       <c r="T33" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U33" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="V33" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W33" s="2" t="s">
-        <v>72</v>
+      <c r="U33" s="2" t="n">
+        <v>154.0</v>
+      </c>
+      <c r="V33" s="2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W33" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="X33" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Y33" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>264</v>
+        <v>121</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H34" s="2" t="n">
         <v>3.0</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>72</v>
@@ -7441,52 +7647,58 @@
       <c r="T34" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U34" s="2" t="b">
+      <c r="U34" s="2" t="n">
+        <v>799.0</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V34" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W34" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X34" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA34" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>268</v>
+        <v>188</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>72</v>
+        <v>251</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H35" s="2" t="n">
         <v>1.0</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>72</v>
@@ -7518,52 +7730,58 @@
       <c r="T35" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U35" s="2" t="b">
+      <c r="U35" s="2" t="n">
+        <v>565.0</v>
+      </c>
+      <c r="V35" s="2" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="W35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V35" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W35" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X35" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z35" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA35" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>271</v>
+        <v>155</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>244</v>
+        <v>192</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H36" s="2" t="n">
         <v>2.0</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>72</v>
@@ -7595,52 +7813,58 @@
       <c r="T36" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U36" s="2" t="b">
+      <c r="U36" s="2" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V36" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W36" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X36" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA36" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>74</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>274</v>
+        <v>125</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>72</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="H37" s="2" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>72</v>
@@ -7672,19 +7896,25 @@
       <c r="T37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="U37" s="2" t="b">
+      <c r="U37" s="2" t="n">
+        <v>759.0</v>
+      </c>
+      <c r="V37" s="2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="W37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="V37" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="W37" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="X37" s="2" t="s">
         <v>72</v>
       </c>
       <c r="Y37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AA37" s="2" t="s">
         <v>72</v>
       </c>
     </row>
@@ -7709,7 +7939,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="10.78515625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.5859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.27734375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.4296875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="15.25" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="17.625" customWidth="true" bestFit="true"/>
@@ -7717,10 +7947,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2"/>
@@ -7729,16 +7959,16 @@
         <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4">
@@ -7778,7 +8008,7 @@
     <row r="6"/>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>36.0</v>
@@ -7884,7 +8114,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -7931,7 +8161,7 @@
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>
@@ -8224,7 +8454,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -8885,8 +9115,8 @@
       <c r="B18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>72</v>
+      <c r="C18" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>72</v>
@@ -9090,8 +9320,8 @@
       <c r="B23" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>284</v>
+      <c r="C23" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>72</v>
@@ -9330,7 +9560,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>84</v>
@@ -9371,13 +9601,13 @@
     </row>
     <row r="3" ht="15.0" customHeight="true">
       <c r="A3" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>72</v>

</xml_diff>